<commit_message>
Made Excel from BOM
</commit_message>
<xml_diff>
--- a/esp32-gps-collar.xlsx
+++ b/esp32-gps-collar.xlsx
@@ -2195,8 +2195,8 @@
   </sheetPr>
   <dimension ref="A1:Z87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="S85" sqref="S85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3921,7 +3921,7 @@
         <v>6</v>
       </c>
       <c r="T31" s="39">
-        <f>G31</f>
+        <f t="shared" ref="T31:T40" si="5">G31</f>
         <v>0</v>
       </c>
       <c r="U31" s="15">
@@ -3972,11 +3972,11 @@
         <v>3</v>
       </c>
       <c r="S32" s="58">
-        <f t="shared" ref="S32:S34" si="5">R32*D32</f>
+        <f t="shared" ref="S32:S34" si="6">R32*D32</f>
         <v>3</v>
       </c>
       <c r="T32" s="39">
-        <f>G32</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U32" s="15">
@@ -4027,11 +4027,11 @@
         <v>4</v>
       </c>
       <c r="S33" s="58">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="T33" s="39">
         <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="T33" s="39">
-        <f>G33</f>
         <v>0</v>
       </c>
       <c r="U33" s="15">
@@ -4082,11 +4082,11 @@
         <v>5</v>
       </c>
       <c r="S34" s="58">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="T34" s="39">
         <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="T34" s="39">
-        <f>G34</f>
         <v>0</v>
       </c>
       <c r="U34" s="15">
@@ -4140,7 +4140,7 @@
       <c r="R35" s="58"/>
       <c r="S35" s="58"/>
       <c r="T35" s="39" t="str">
-        <f>G35</f>
+        <f t="shared" si="5"/>
         <v>11,75</v>
       </c>
       <c r="U35" s="15">
@@ -4194,7 +4194,7 @@
       <c r="R36" s="58"/>
       <c r="S36" s="58"/>
       <c r="T36" s="39" t="str">
-        <f>G36</f>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="U36" s="15">
@@ -4248,7 +4248,7 @@
       <c r="R37" s="58"/>
       <c r="S37" s="58"/>
       <c r="T37" s="39" t="str">
-        <f>G37</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="U37" s="15">
@@ -4302,7 +4302,7 @@
       <c r="R38" s="58"/>
       <c r="S38" s="58"/>
       <c r="T38" s="39" t="str">
-        <f>G38</f>
+        <f t="shared" si="5"/>
         <v>6,25</v>
       </c>
       <c r="U38" s="15">
@@ -4354,7 +4354,7 @@
       <c r="R39" s="58"/>
       <c r="S39" s="58"/>
       <c r="T39" s="39">
-        <f>G39</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U39" s="15">
@@ -4408,7 +4408,7 @@
       <c r="R40" s="58"/>
       <c r="S40" s="58"/>
       <c r="T40" s="39" t="str">
-        <f>G40</f>
+        <f t="shared" si="5"/>
         <v>57,5</v>
       </c>
       <c r="U40" s="15">
@@ -5073,7 +5073,7 @@
       <c r="R52" s="58"/>
       <c r="S52" s="58"/>
       <c r="T52" s="37" t="str">
-        <f t="shared" ref="T52:T53" si="6">I52</f>
+        <f t="shared" ref="T52:T53" si="7">I52</f>
         <v>0,06</v>
       </c>
       <c r="U52" s="15">
@@ -5127,7 +5127,7 @@
       <c r="R53" s="58"/>
       <c r="S53" s="58"/>
       <c r="T53" s="37" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0,07</v>
       </c>
       <c r="U53" s="15">
@@ -5179,7 +5179,7 @@
       <c r="R54" s="58"/>
       <c r="S54" s="58"/>
       <c r="T54" s="39">
-        <f>G54</f>
+        <f t="shared" ref="T54:T62" si="8">G54</f>
         <v>0</v>
       </c>
       <c r="U54" s="15">
@@ -5235,7 +5235,7 @@
       <c r="R55" s="58"/>
       <c r="S55" s="58"/>
       <c r="T55" s="39">
-        <f>G55</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U55" s="15">
@@ -5289,7 +5289,7 @@
       <c r="R56" s="58"/>
       <c r="S56" s="58"/>
       <c r="T56" s="39">
-        <f>G56</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U56" s="15">
@@ -5345,7 +5345,7 @@
       <c r="R57" s="58"/>
       <c r="S57" s="58"/>
       <c r="T57" s="39">
-        <f>G57</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U57" s="15">
@@ -5399,7 +5399,7 @@
       <c r="R58" s="58"/>
       <c r="S58" s="58"/>
       <c r="T58" s="39">
-        <f>G58</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U58" s="15">
@@ -5451,7 +5451,7 @@
       <c r="R59" s="58"/>
       <c r="S59" s="58"/>
       <c r="T59" s="39">
-        <f>G59</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U59" s="15">
@@ -5505,7 +5505,7 @@
       <c r="R60" s="58"/>
       <c r="S60" s="58"/>
       <c r="T60" s="39">
-        <f>G60</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U60" s="15">
@@ -5557,7 +5557,7 @@
       <c r="R61" s="58"/>
       <c r="S61" s="58"/>
       <c r="T61" s="39">
-        <f>G61</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U61" s="15">
@@ -5609,7 +5609,7 @@
       <c r="R62" s="58"/>
       <c r="S62" s="58"/>
       <c r="T62" s="39">
-        <f>G62</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U62" s="15">
@@ -5907,7 +5907,7 @@
         <v>1</v>
       </c>
       <c r="X67" s="16">
-        <f t="shared" ref="X67:X81" si="7">W67*T67</f>
+        <f t="shared" ref="X67:X81" si="9">W67*T67</f>
         <v>2.25</v>
       </c>
       <c r="Y67" s="34"/>
@@ -5949,19 +5949,19 @@
         <v>0,75</v>
       </c>
       <c r="U68" s="15">
-        <f t="shared" ref="U68:U81" si="8">D68</f>
+        <f t="shared" ref="U68:U81" si="10">D68</f>
         <v>1</v>
       </c>
       <c r="V68" s="14">
-        <f t="shared" ref="V68:V82" si="9">U68*T68</f>
+        <f t="shared" ref="V68:V82" si="11">U68*T68</f>
         <v>0.75</v>
       </c>
       <c r="W68" s="15">
-        <f t="shared" ref="W68:W81" si="10">U68</f>
+        <f t="shared" ref="W68:W81" si="12">U68</f>
         <v>1</v>
       </c>
       <c r="X68" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.75</v>
       </c>
       <c r="Y68" s="34"/>
@@ -6009,19 +6009,19 @@
         <v>64.394999999999996</v>
       </c>
       <c r="U69" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="V69" s="14">
+        <f t="shared" si="11"/>
+        <v>64.394999999999996</v>
+      </c>
+      <c r="W69" s="15">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="X69" s="16">
         <f t="shared" si="9"/>
-        <v>64.394999999999996</v>
-      </c>
-      <c r="W69" s="15">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="X69" s="16">
-        <f t="shared" si="7"/>
         <v>64.394999999999996</v>
       </c>
       <c r="Y69" s="34"/>
@@ -6065,19 +6065,19 @@
         <v>0,06</v>
       </c>
       <c r="U70" s="15">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="V70" s="14">
-        <f t="shared" si="9"/>
-        <v>0.6</v>
-      </c>
-      <c r="W70" s="15">
         <f t="shared" si="10"/>
         <v>10</v>
       </c>
+      <c r="V70" s="14">
+        <f t="shared" si="11"/>
+        <v>0.6</v>
+      </c>
+      <c r="W70" s="15">
+        <f t="shared" si="12"/>
+        <v>10</v>
+      </c>
       <c r="X70" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.6</v>
       </c>
       <c r="Y70" s="34"/>
@@ -6119,18 +6119,18 @@
         <v>75,75</v>
       </c>
       <c r="U71" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="V71" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>75.75</v>
       </c>
       <c r="W71" s="15">
         <v>0</v>
       </c>
       <c r="X71" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Y71" s="34"/>
@@ -6182,19 +6182,19 @@
         <v>253,84</v>
       </c>
       <c r="U72" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="V72" s="14">
+        <f t="shared" si="11"/>
+        <v>253.84</v>
+      </c>
+      <c r="W72" s="15">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="X72" s="16">
         <f t="shared" si="9"/>
-        <v>253.84</v>
-      </c>
-      <c r="W72" s="15">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="X72" s="16">
-        <f t="shared" si="7"/>
         <v>253.84</v>
       </c>
       <c r="Y72" s="34"/>
@@ -6236,19 +6236,19 @@
         <v>45</v>
       </c>
       <c r="U73" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="V73" s="14">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="W73" s="15">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="X73" s="16">
         <f t="shared" si="9"/>
-        <v>45</v>
-      </c>
-      <c r="W73" s="15">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="X73" s="16">
-        <f t="shared" si="7"/>
         <v>45</v>
       </c>
       <c r="Y73" s="34"/>
@@ -6291,19 +6291,19 @@
         <v>0</v>
       </c>
       <c r="U74" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="V74" s="14">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="W74" s="15">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="X74" s="16">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="W74" s="15">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="X74" s="16">
-        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y74" s="34"/>
@@ -6345,19 +6345,19 @@
         <v>1,25</v>
       </c>
       <c r="U75" s="15">
-        <f t="shared" si="8"/>
-        <v>4</v>
-      </c>
-      <c r="V75" s="14">
-        <f t="shared" si="9"/>
-        <v>5</v>
-      </c>
-      <c r="W75" s="15">
         <f t="shared" si="10"/>
         <v>4</v>
       </c>
+      <c r="V75" s="14">
+        <f t="shared" si="11"/>
+        <v>5</v>
+      </c>
+      <c r="W75" s="15">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
       <c r="X75" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="Y75" s="34"/>
@@ -6399,19 +6399,19 @@
         <v>0,5</v>
       </c>
       <c r="U76" s="15">
-        <f t="shared" si="8"/>
-        <v>4</v>
-      </c>
-      <c r="V76" s="14">
-        <f t="shared" si="9"/>
-        <v>2</v>
-      </c>
-      <c r="W76" s="15">
         <f t="shared" si="10"/>
         <v>4</v>
       </c>
+      <c r="V76" s="14">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="W76" s="15">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
       <c r="X76" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="Y76" s="34"/>
@@ -6455,16 +6455,16 @@
         <v>91.367999999999995</v>
       </c>
       <c r="U77" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="V77" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>91.367999999999995</v>
       </c>
       <c r="W77" s="15"/>
       <c r="X77" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Y77" s="34"/>
@@ -6506,19 +6506,19 @@
         <v>64</v>
       </c>
       <c r="U78" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="V78" s="14">
+        <f t="shared" si="11"/>
+        <v>64</v>
+      </c>
+      <c r="W78" s="15">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="X78" s="16">
         <f t="shared" si="9"/>
-        <v>64</v>
-      </c>
-      <c r="W78" s="15">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="X78" s="16">
-        <f t="shared" si="7"/>
         <v>64</v>
       </c>
       <c r="Y78" s="34"/>
@@ -6560,19 +6560,19 @@
         <v>6,75</v>
       </c>
       <c r="U79" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="V79" s="14">
+        <f t="shared" si="11"/>
+        <v>6.75</v>
+      </c>
+      <c r="W79" s="15">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="X79" s="16">
         <f t="shared" si="9"/>
-        <v>6.75</v>
-      </c>
-      <c r="W79" s="15">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="X79" s="16">
-        <f t="shared" si="7"/>
         <v>6.75</v>
       </c>
       <c r="Y79" s="34"/>
@@ -6615,19 +6615,19 @@
         <v>0</v>
       </c>
       <c r="U80" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="V80" s="14">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="W80" s="15">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="X80" s="16">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="W80" s="15">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="X80" s="16">
-        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y80" s="34"/>
@@ -6669,19 +6669,19 @@
         <v>4,25</v>
       </c>
       <c r="U81" s="23">
-        <f t="shared" si="8"/>
-        <v>3</v>
-      </c>
-      <c r="V81" s="33">
-        <f t="shared" si="9"/>
-        <v>12.75</v>
-      </c>
-      <c r="W81" s="23">
         <f t="shared" si="10"/>
         <v>3</v>
       </c>
+      <c r="V81" s="33">
+        <f t="shared" si="11"/>
+        <v>12.75</v>
+      </c>
+      <c r="W81" s="23">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
       <c r="X81" s="24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>12.75</v>
       </c>
       <c r="Y81" s="34"/>
@@ -6708,15 +6708,15 @@
         <v>0.8</v>
       </c>
       <c r="V82" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.64000000000000012</v>
       </c>
       <c r="W82" s="9">
-        <f t="shared" ref="W82" si="11">U82</f>
+        <f t="shared" ref="W82" si="13">U82</f>
         <v>0.8</v>
       </c>
       <c r="X82" s="9">
-        <f t="shared" ref="X82" si="12">W82*T82</f>
+        <f t="shared" ref="X82" si="14">W82*T82</f>
         <v>0.64000000000000012</v>
       </c>
       <c r="Y82" s="34"/>
@@ -6747,7 +6747,7 @@
       </c>
       <c r="W84" s="75"/>
       <c r="X84" s="75">
-        <f t="shared" ref="W84:X84" si="13">SUM(X1:X82)</f>
+        <f t="shared" ref="X84" si="15">SUM(X1:X82)</f>
         <v>1867.4959999999992</v>
       </c>
     </row>
@@ -6763,7 +6763,7 @@
         <v>358</v>
       </c>
       <c r="S85" s="73">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="U85" s="9" t="s">
         <v>362</v>
@@ -6773,7 +6773,7 @@
         <v>157.06855999999999</v>
       </c>
       <c r="X85" s="9">
-        <f t="shared" ref="W85:X85" si="14">X84/25</f>
+        <f t="shared" ref="X85" si="16">X84/25</f>
         <v>74.699839999999966</v>
       </c>
     </row>
@@ -6783,7 +6783,7 @@
       </c>
       <c r="V86" s="76">
         <f>(V84*S84)+(X84*S85)</f>
-        <v>15323.411999999997</v>
+        <v>11588.419999999998</v>
       </c>
     </row>
     <row r="87" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
@@ -6792,7 +6792,7 @@
       </c>
       <c r="V87" s="76">
         <f>V86/24.3</f>
-        <v>630.59308641975292</v>
+        <v>476.88971193415631</v>
       </c>
     </row>
   </sheetData>

</xml_diff>